<commit_message>
Added results for n=19
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\QED\submission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB76531D-5012-4207-9668-62CB36D882BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83643302-4914-4150-873B-DD01A6053CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="806" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="806" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="n-queens tilings" sheetId="23" r:id="rId1"/>
@@ -31,6 +31,7 @@
     <sheet name="14" sheetId="15" r:id="rId16"/>
     <sheet name="15" sheetId="16" r:id="rId17"/>
     <sheet name="18" sheetId="20" r:id="rId18"/>
+    <sheet name="19" sheetId="24" r:id="rId19"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="21">
   <si>
     <t>N</t>
   </si>
@@ -120,7 +121,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -148,13 +149,6 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -200,7 +194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -212,23 +206,20 @@
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1419,7 +1410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57CC072-04CF-49B5-A34E-16C154FDD97F}">
   <dimension ref="A3:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1634,11 +1625,18 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B22" s="8"/>
-      <c r="C22" s="7"/>
+      <c r="A22" s="4">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4">
+        <v>4968057848</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B23" s="8"/>
+      <c r="B23" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1933,10 +1931,10 @@
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="10"/>
+      <c r="D2" s="14"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -3046,101 +3044,101 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="12.5703125" style="12"/>
+    <col min="1" max="1" width="14" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="12.5703125" style="9"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3" s="9">
         <v>12</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="10">
         <v>14200</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="10">
         <v>12996</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="12">
-        <v>8</v>
-      </c>
-      <c r="C6" s="12">
+      <c r="B6" s="9">
+        <v>8</v>
+      </c>
+      <c r="C6" s="9">
         <v>68</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="9">
         <v>64</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="10">
         <v>602</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="A7" s="9">
         <v>6</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="9">
         <v>6</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="9">
         <v>66</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="9">
         <v>66</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="10">
         <v>12996</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
-        <v>8</v>
-      </c>
-      <c r="B8" s="12">
+      <c r="A8" s="9">
+        <v>8</v>
+      </c>
+      <c r="B8" s="9">
         <v>4</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="9">
         <v>64</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="9">
         <v>68</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="10">
         <v>602</v>
       </c>
     </row>
@@ -3163,122 +3161,122 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="12.5703125" style="12"/>
+    <col min="1" max="1" width="14" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="12.5703125" style="9"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3" s="9">
         <v>13</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="10">
         <v>73712</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="10">
         <v>58392</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="9">
         <v>3</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="9">
         <v>10</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="9">
         <v>82</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="9">
         <v>74</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="10">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="A7" s="9">
         <v>5</v>
       </c>
-      <c r="B7" s="12">
-        <v>8</v>
-      </c>
-      <c r="C7" s="12">
+      <c r="B7" s="9">
+        <v>8</v>
+      </c>
+      <c r="C7" s="9">
         <v>80</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="9">
         <v>76</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="10">
         <v>14256</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="9">
         <v>7</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="9">
         <v>6</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="9">
         <v>78</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="9">
         <v>78</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="10">
         <v>58392</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="A9" s="9">
         <v>9</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="9">
         <v>4</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="9">
         <v>76</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="9">
         <v>80</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="10">
         <v>1048</v>
       </c>
     </row>
@@ -3300,135 +3298,134 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="12.5703125" style="12"/>
+    <col min="1" max="1" width="14" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="12.5703125" style="9"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="17"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
+      <c r="A3" s="11">
         <v>14</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="11">
         <v>365596</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
+      <c r="A6" s="11">
         <v>4</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="11">
         <v>10</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="11">
         <v>94</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="11">
         <v>88</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="12">
         <v>478</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
+      <c r="A7" s="11">
         <v>6</v>
       </c>
-      <c r="B7" s="14">
-        <v>8</v>
-      </c>
-      <c r="C7" s="14">
+      <c r="B7" s="11">
+        <v>8</v>
+      </c>
+      <c r="C7" s="11">
         <v>92</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="11">
         <v>90</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="12">
         <v>182320</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
-        <v>8</v>
-      </c>
-      <c r="B8" s="14">
+      <c r="A8" s="11">
+        <v>8</v>
+      </c>
+      <c r="B8" s="11">
         <v>6</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="11">
         <v>90</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="11">
         <v>92</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="12">
         <v>182320</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
+      <c r="A9" s="11">
         <v>10</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="11">
         <v>4</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="11">
         <v>88</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="11">
         <v>94</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="12">
         <v>478</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="11" t="s">
+      <c r="A11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14">
+      <c r="A12" s="11">
         <v>0</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="12">
         <v>365596</v>
       </c>
     </row>
@@ -3626,118 +3623,118 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="14" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3" s="9">
         <v>18</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="10">
         <v>666090624</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="9">
         <v>6</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="9">
         <v>12</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="9">
         <v>156</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="9">
         <v>150</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="10">
         <v>3818084</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
-        <v>8</v>
-      </c>
-      <c r="B7" s="12">
+      <c r="A7" s="9">
+        <v>8</v>
+      </c>
+      <c r="B7" s="9">
         <v>10</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="9">
         <v>154</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="9">
         <v>152</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="10">
         <v>329227228</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="9">
         <v>10</v>
       </c>
-      <c r="B8" s="12">
-        <v>8</v>
-      </c>
-      <c r="C8" s="12">
+      <c r="B8" s="9">
+        <v>8</v>
+      </c>
+      <c r="C8" s="9">
         <v>152</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="9">
         <v>154</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="10">
         <v>329227228</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="A9" s="9">
         <v>12</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="9">
         <v>6</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="9">
         <v>150</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="9">
         <v>156</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="10">
         <v>3818084</v>
       </c>
     </row>
@@ -3747,9 +3744,166 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94DD5D2A-62F5-4668-A501-91DA4E1634B4}">
+  <dimension ref="A2:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>19</v>
+      </c>
+      <c r="B3" s="10">
+        <v>4968057848</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9">
+        <v>14</v>
+      </c>
+      <c r="C6" s="9">
+        <v>176</v>
+      </c>
+      <c r="D6" s="9">
+        <v>166</v>
+      </c>
+      <c r="E6" s="10">
+        <v>26296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>7</v>
+      </c>
+      <c r="B7" s="9">
+        <v>12</v>
+      </c>
+      <c r="C7" s="9">
+        <v>174</v>
+      </c>
+      <c r="D7" s="9">
+        <v>168</v>
+      </c>
+      <c r="E7" s="10">
+        <v>156210840</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>9</v>
+      </c>
+      <c r="B8" s="9">
+        <v>10</v>
+      </c>
+      <c r="C8" s="9">
+        <v>172</v>
+      </c>
+      <c r="D8" s="9">
+        <v>170</v>
+      </c>
+      <c r="E8" s="10">
+        <v>3508201080</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>11</v>
+      </c>
+      <c r="B9" s="9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="9">
+        <v>170</v>
+      </c>
+      <c r="D9" s="9">
+        <v>172</v>
+      </c>
+      <c r="E9" s="10">
+        <v>1298380976</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>13</v>
+      </c>
+      <c r="B10" s="9">
+        <v>6</v>
+      </c>
+      <c r="C10" s="9">
+        <v>168</v>
+      </c>
+      <c r="D10" s="9">
+        <v>174</v>
+      </c>
+      <c r="E10" s="10">
+        <v>5238656</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61870D5-A3B9-47B8-B536-6E843C410BB5}">
-  <dimension ref="A3:B21"/>
+  <dimension ref="A3:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -3757,8 +3911,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" customWidth="1"/>
-    <col min="2" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3911,6 +4066,14 @@
       </c>
       <c r="B21" s="4">
         <v>666090624</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4">
+        <v>4968057848</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some more data points
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\QED\submission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83643302-4914-4150-873B-DD01A6053CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A928C69-7061-4A16-953C-33D3A0921921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="806" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,8 +30,10 @@
     <sheet name="13" sheetId="14" r:id="rId15"/>
     <sheet name="14" sheetId="15" r:id="rId16"/>
     <sheet name="15" sheetId="16" r:id="rId17"/>
-    <sheet name="18" sheetId="20" r:id="rId18"/>
-    <sheet name="19" sheetId="24" r:id="rId19"/>
+    <sheet name="16" sheetId="25" r:id="rId18"/>
+    <sheet name="17" sheetId="26" r:id="rId19"/>
+    <sheet name="18" sheetId="20" r:id="rId20"/>
+    <sheet name="19" sheetId="24" r:id="rId21"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="21">
   <si>
     <t>N</t>
   </si>
@@ -121,7 +123,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -172,6 +174,11 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -194,7 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -216,6 +223,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1417,6 +1427,7 @@
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1602,7 +1613,9 @@
       <c r="B19" s="4">
         <v>14772512</v>
       </c>
-      <c r="C19" s="4"/>
+      <c r="C19" s="13">
+        <v>12486228</v>
+      </c>
     </row>
     <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
@@ -1611,7 +1624,9 @@
       <c r="B20" s="4">
         <v>95815104</v>
       </c>
-      <c r="C20" s="4"/>
+      <c r="C20" s="13">
+        <v>70637480</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
@@ -1640,6 +1655,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1931,10 +1947,10 @@
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
+      <c r="D2" s="15"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -3321,7 +3337,7 @@
       <c r="A3" s="11">
         <v>14</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="10">
         <v>365596</v>
       </c>
       <c r="C3" s="11">
@@ -3614,139 +3630,179 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25F21330-9009-4846-A18D-009B42D39CDA}">
-  <dimension ref="A2:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B84C5BE-354A-44F5-A0A9-70207E51736D}">
+  <dimension ref="A2:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
-        <v>18</v>
+      <c r="D2" s="2"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>16</v>
       </c>
       <c r="B3" s="10">
-        <v>666090624</v>
-      </c>
-      <c r="C3" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+        <v>14772512</v>
+      </c>
+      <c r="C3" s="10">
+        <v>12486228</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3">
+        <v>124</v>
+      </c>
+      <c r="D6" s="3">
+        <v>116</v>
+      </c>
+      <c r="E6" s="4">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B7" s="3">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3">
+        <v>122</v>
+      </c>
+      <c r="D7" s="3">
+        <v>118</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1143066</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3">
+        <v>120</v>
+      </c>
+      <c r="D8" s="3">
+        <v>120</v>
+      </c>
+      <c r="E8" s="4">
+        <v>12486228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3">
+        <v>118</v>
+      </c>
+      <c r="D9" s="3">
+        <v>122</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1143066</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>12</v>
       </c>
-      <c r="C6" s="9">
-        <v>156</v>
-      </c>
-      <c r="D6" s="9">
-        <v>150</v>
-      </c>
-      <c r="E6" s="10">
-        <v>3818084</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <v>8</v>
-      </c>
-      <c r="B7" s="9">
-        <v>10</v>
-      </c>
-      <c r="C7" s="9">
-        <v>154</v>
-      </c>
-      <c r="D7" s="9">
-        <v>152</v>
-      </c>
-      <c r="E7" s="10">
-        <v>329227228</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
-        <v>10</v>
-      </c>
-      <c r="B8" s="9">
-        <v>8</v>
-      </c>
-      <c r="C8" s="9">
-        <v>152</v>
-      </c>
-      <c r="D8" s="9">
-        <v>154</v>
-      </c>
-      <c r="E8" s="10">
-        <v>329227228</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
-        <v>12</v>
-      </c>
-      <c r="B9" s="9">
-        <v>6</v>
-      </c>
-      <c r="C9" s="9">
-        <v>150</v>
-      </c>
-      <c r="D9" s="9">
-        <v>156</v>
-      </c>
-      <c r="E9" s="10">
-        <v>3818084</v>
-      </c>
+      <c r="B10" s="1">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>116</v>
+      </c>
+      <c r="D10" s="1">
+        <v>124</v>
+      </c>
+      <c r="E10" s="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94DD5D2A-62F5-4668-A501-91DA4E1634B4}">
-  <dimension ref="A2:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{203BC081-B8AB-43A6-A04D-F704840D7A1F}">
+  <dimension ref="A2:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3755,10 +3811,10 @@
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -3776,13 +3832,13 @@
     </row>
     <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="10">
-        <v>4968057848</v>
-      </c>
-      <c r="C3" s="9">
-        <v>0</v>
+        <v>95815104</v>
+      </c>
+      <c r="C3" s="10">
+        <v>70637480</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -3816,16 +3872,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="9">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="9">
-        <v>176</v>
+        <v>140</v>
       </c>
       <c r="D6" s="9">
-        <v>166</v>
+        <v>132</v>
       </c>
       <c r="E6" s="10">
-        <v>26296</v>
+        <v>43736</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -3833,16 +3889,16 @@
         <v>7</v>
       </c>
       <c r="B7" s="9">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="9">
-        <v>174</v>
+        <v>138</v>
       </c>
       <c r="D7" s="9">
-        <v>168</v>
+        <v>134</v>
       </c>
       <c r="E7" s="10">
-        <v>156210840</v>
+        <v>22895000</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -3850,16 +3906,16 @@
         <v>9</v>
       </c>
       <c r="B8" s="9">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" s="9">
-        <v>172</v>
+        <v>136</v>
       </c>
       <c r="D8" s="9">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="E8" s="10">
-        <v>3508201080</v>
+        <v>70637480</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -3867,16 +3923,16 @@
         <v>11</v>
       </c>
       <c r="B9" s="9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" s="9">
-        <v>170</v>
+        <v>134</v>
       </c>
       <c r="D9" s="9">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="E9" s="10">
-        <v>1298380976</v>
+        <v>2238800</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -3884,17 +3940,24 @@
         <v>13</v>
       </c>
       <c r="B10" s="9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C10" s="9">
-        <v>168</v>
+        <v>132</v>
       </c>
       <c r="D10" s="9">
-        <v>174</v>
-      </c>
-      <c r="E10" s="10">
-        <v>5238656</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="E10" s="9">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4079,6 +4142,294 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25F21330-9009-4846-A18D-009B42D39CDA}">
+  <dimension ref="A2:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>18</v>
+      </c>
+      <c r="B3" s="10">
+        <v>666090624</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>6</v>
+      </c>
+      <c r="B6" s="9">
+        <v>12</v>
+      </c>
+      <c r="C6" s="9">
+        <v>156</v>
+      </c>
+      <c r="D6" s="9">
+        <v>150</v>
+      </c>
+      <c r="E6" s="10">
+        <v>3818084</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>8</v>
+      </c>
+      <c r="B7" s="9">
+        <v>10</v>
+      </c>
+      <c r="C7" s="9">
+        <v>154</v>
+      </c>
+      <c r="D7" s="9">
+        <v>152</v>
+      </c>
+      <c r="E7" s="10">
+        <v>329227228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9">
+        <v>8</v>
+      </c>
+      <c r="C8" s="9">
+        <v>152</v>
+      </c>
+      <c r="D8" s="9">
+        <v>154</v>
+      </c>
+      <c r="E8" s="10">
+        <v>329227228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>12</v>
+      </c>
+      <c r="B9" s="9">
+        <v>6</v>
+      </c>
+      <c r="C9" s="9">
+        <v>150</v>
+      </c>
+      <c r="D9" s="9">
+        <v>156</v>
+      </c>
+      <c r="E9" s="10">
+        <v>3818084</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94DD5D2A-62F5-4668-A501-91DA4E1634B4}">
+  <dimension ref="A2:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>19</v>
+      </c>
+      <c r="B3" s="10">
+        <v>4968057848</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9">
+        <v>14</v>
+      </c>
+      <c r="C6" s="9">
+        <v>176</v>
+      </c>
+      <c r="D6" s="9">
+        <v>166</v>
+      </c>
+      <c r="E6" s="10">
+        <v>26296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>7</v>
+      </c>
+      <c r="B7" s="9">
+        <v>12</v>
+      </c>
+      <c r="C7" s="9">
+        <v>174</v>
+      </c>
+      <c r="D7" s="9">
+        <v>168</v>
+      </c>
+      <c r="E7" s="10">
+        <v>156210840</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>9</v>
+      </c>
+      <c r="B8" s="9">
+        <v>10</v>
+      </c>
+      <c r="C8" s="9">
+        <v>172</v>
+      </c>
+      <c r="D8" s="9">
+        <v>170</v>
+      </c>
+      <c r="E8" s="10">
+        <v>3508201080</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>11</v>
+      </c>
+      <c r="B9" s="9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="9">
+        <v>170</v>
+      </c>
+      <c r="D9" s="9">
+        <v>172</v>
+      </c>
+      <c r="E9" s="10">
+        <v>1298380976</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>13</v>
+      </c>
+      <c r="B10" s="9">
+        <v>6</v>
+      </c>
+      <c r="C10" s="9">
+        <v>168</v>
+      </c>
+      <c r="D10" s="9">
+        <v>174</v>
+      </c>
+      <c r="E10" s="10">
+        <v>5238656</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>